<commit_message>
perbaikan file untuk import sementara
</commit_message>
<xml_diff>
--- a/public/template/template_donasi.xlsx
+++ b/public/template/template_donasi.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>tanggal</t>
   </si>
@@ -111,61 +111,7 @@
     <t>angkatan</t>
   </si>
   <si>
-    <t>2015-06-12</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>John Doe Two</t>
-  </si>
-  <si>
-    <t>STI 2007</t>
-  </si>
-  <si>
-    <t>ITB '98</t>
-  </si>
-  <si>
-    <t>BPUDL</t>
-  </si>
-  <si>
-    <t>PT. Freeport</t>
-  </si>
-  <si>
-    <t>Manajemen</t>
-  </si>
-  <si>
-    <t>STI</t>
-  </si>
-  <si>
-    <t>Jane Doe</t>
-  </si>
-  <si>
-    <t>Elektro</t>
-  </si>
-  <si>
-    <t>Elektro '99</t>
-  </si>
-  <si>
-    <t>Suprapto</t>
-  </si>
-  <si>
-    <t>Shintiya</t>
-  </si>
-  <si>
-    <t>Fauzan</t>
-  </si>
-  <si>
-    <t>1 kali</t>
-  </si>
-  <si>
-    <t>Untuk prodi x</t>
-  </si>
-  <si>
-    <t>Bandung</t>
-  </si>
-  <si>
-    <t>Jakarta</t>
+    <t>Kolom program_studi dan angkatan diisi jika jenis donatur adalah Alumni</t>
   </si>
 </sst>
 </file>
@@ -534,13 +480,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,281 +546,41 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
-        <v>11000000</v>
-      </c>
-      <c r="H2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>48</v>
-      </c>
       <c r="M2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3">
-        <v>2009</v>
-      </c>
-      <c r="G3">
-        <v>12000000</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" t="s">
-        <v>49</v>
-      </c>
       <c r="M3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4">
-        <v>2007</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4">
-        <v>21000000</v>
-      </c>
-      <c r="H4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L4" t="s">
-        <v>48</v>
-      </c>
       <c r="M4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <v>60000000</v>
-      </c>
-      <c r="H5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" t="s">
-        <v>49</v>
-      </c>
       <c r="M5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6">
-        <v>22000000</v>
-      </c>
-      <c r="H6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" t="s">
-        <v>48</v>
-      </c>
       <c r="N6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7">
-        <v>90000000</v>
-      </c>
-      <c r="H7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" t="s">
-        <v>49</v>
-      </c>
       <c r="N7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8">
-        <v>107</v>
-      </c>
-      <c r="E8">
-        <v>2001</v>
-      </c>
-      <c r="G8">
-        <v>12000000</v>
-      </c>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" t="s">
-        <v>48</v>
-      </c>
       <c r="N8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9">
-        <v>1999</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9">
-        <v>80000000</v>
-      </c>
-      <c r="H9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" t="s">
-        <v>49</v>
-      </c>
       <c r="N9" t="s">
         <v>16</v>
       </c>
@@ -914,19 +620,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N19" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>